<commit_message>
I have updated the design doc and the acceptance test plan. - Daniel Pittman
</commit_message>
<xml_diff>
--- a/docs/Acceptance Test Plan.xlsx
+++ b/docs/Acceptance Test Plan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="151">
   <si>
     <t>Instructions</t>
   </si>
@@ -463,6 +463,18 @@
   </si>
   <si>
     <t>Given I have not entered text into the search bar, When I click on no type buttons, then all pokemon will appear</t>
+  </si>
+  <si>
+    <t>As a User I want to see my past order history so that I have receipts of all the purchases I have made to keep track of purchases and protect against fraudulent or accidental purchases.</t>
+  </si>
+  <si>
+    <t>Given I am a user and I have purchased one or more orders of goods when I go to my order history in my user profile then I expect to see a list of all my orders and what I purchased.</t>
+  </si>
+  <si>
+    <t>DP;11/13/22; Looks good and it works!</t>
+  </si>
+  <si>
+    <t>Given I am a user and I have not purchased any orders when I go to my order history in my user profile then I expect to not see any past orders.</t>
   </si>
 </sst>
 </file>
@@ -6496,8 +6508,8 @@
       <c r="Z73" s="14"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="2"/>
-      <c r="B74" s="12" t="s">
+      <c r="A74" s="29"/>
+      <c r="B74" s="30" t="s">
         <v>146</v>
       </c>
       <c r="C74" s="13"/>
@@ -6530,12 +6542,20 @@
       <c r="Z74" s="14"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
+      <c r="A75" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>148</v>
+      </c>
       <c r="C75" s="13"/>
       <c r="D75" s="2"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="2"/>
+      <c r="E75" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
@@ -6558,12 +6578,18 @@
       <c r="Z75" s="14"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
+      <c r="A76" s="29"/>
+      <c r="B76" s="30" t="s">
+        <v>150</v>
+      </c>
       <c r="C76" s="13"/>
       <c r="D76" s="2"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="2"/>
+      <c r="E76" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>149</v>
+      </c>
       <c r="G76" s="14"/>
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>

</xml_diff>